<commit_message>
issue state column was updated
</commit_message>
<xml_diff>
--- a/analyzed_issues.xlsx
+++ b/analyzed_issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Ulthar-systems\barrack-studio\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E79D7E-0339-4CA4-8AC9-40B6FEFC1D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845B3534-19A5-433D-B2C8-41FE6A5AB7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="2730" windowWidth="17775" windowHeight="10455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="915" windowWidth="22650" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyzed Issues" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="203">
   <si>
     <t>issue_id</t>
   </si>
@@ -41,9 +41,6 @@
     <t>issue_url</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>5369</t>
   </si>
   <si>
@@ -618,13 +615,28 @@
   </si>
   <si>
     <t>https://github.com/facebook/react/issues/24160-</t>
+  </si>
+  <si>
+    <t>issue_files</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>issue_pr_url</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>issue_state</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +648,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -662,9 +682,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -968,20 +989,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="5" max="5" width="54.7109375" customWidth="1"/>
-    <col min="6" max="6" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="54.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -998,1114 +1023,1425 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>201</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>201</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>60</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
+        <v>201</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>66</v>
       </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>68</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>70</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>201</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D18" t="s">
         <v>77</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
         <v>68</v>
       </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>201</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
         <v>89</v>
       </c>
-      <c r="B21" t="s">
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
         <v>68</v>
       </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>94</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>97</v>
-      </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
         <v>99</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
         <v>103</v>
       </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
         <v>107</v>
       </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>108</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
         <v>111</v>
       </c>
-      <c r="B26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>112</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
+        <v>201</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" t="s">
         <v>115</v>
       </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>116</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
+        <v>201</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
         <v>119</v>
       </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>120</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
         <v>123</v>
       </c>
-      <c r="B29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>124</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>201</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
         <v>127</v>
       </c>
-      <c r="B30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>128</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>201</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="H30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
         <v>131</v>
       </c>
-      <c r="B31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>132</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>201</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" t="s">
         <v>135</v>
       </c>
-      <c r="B32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>136</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
+        <v>201</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="H32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
         <v>139</v>
       </c>
-      <c r="B33" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>140</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" t="s">
+        <v>201</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35" t="s">
+        <v>201</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" t="s">
+        <v>201</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" t="s">
+        <v>201</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" t="s">
+        <v>201</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" t="s">
+        <v>201</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" t="s">
+        <v>201</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" t="s">
+        <v>201</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" t="s">
+        <v>201</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" t="s">
+        <v>156</v>
+      </c>
+      <c r="F43" t="s">
+        <v>201</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" t="s">
+        <v>201</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" t="s">
-        <v>143</v>
-      </c>
-      <c r="E34" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" t="s">
-        <v>145</v>
-      </c>
-      <c r="E35" t="s">
-        <v>146</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" t="s">
-        <v>148</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" t="s">
-        <v>149</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B39" t="s">
-        <v>98</v>
-      </c>
-      <c r="C39" t="s">
-        <v>99</v>
-      </c>
-      <c r="D39" t="s">
-        <v>150</v>
-      </c>
-      <c r="E39" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" t="s">
-        <v>124</v>
-      </c>
-      <c r="E40" t="s">
-        <v>152</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" t="s">
-        <v>155</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>139</v>
-      </c>
-      <c r="B44" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" t="s">
-        <v>140</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="H44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>158</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s">
         <v>159</v>
       </c>
-      <c r="B45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>160</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
+        <v>201</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="H45" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s">
         <v>163</v>
       </c>
-      <c r="B46" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>164</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
+        <v>201</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="H46" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
         <v>167</v>
       </c>
-      <c r="B47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>168</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
+        <v>201</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="H47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" t="s">
         <v>171</v>
       </c>
-      <c r="B48" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>172</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="H48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" t="s">
         <v>175</v>
       </c>
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>176</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
+        <v>201</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="H49" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" t="s">
         <v>179</v>
       </c>
-      <c r="B50" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>180</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
+        <v>201</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="H50" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="s">
         <v>183</v>
       </c>
-      <c r="B51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>184</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
+        <v>201</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="H51" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" t="s">
         <v>187</v>
       </c>
-      <c r="B52" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>188</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
+        <v>201</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="H52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" t="s">
         <v>191</v>
       </c>
-      <c r="B53" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" t="s">
-        <v>99</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>192</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
+        <v>201</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>194</v>
+      <c r="H53" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F23" r:id="rId19" xr:uid="{90527381-36DF-4A90-999E-72A67B889E6C}"/>
-    <hyperlink ref="F24" r:id="rId20" xr:uid="{1EF029AC-4F76-4CBB-8667-8BC81D53A3DF}"/>
-    <hyperlink ref="F26" r:id="rId21" xr:uid="{36D72442-02B1-43AE-9099-FA35E2EF38CE}"/>
-    <hyperlink ref="F25" r:id="rId22" xr:uid="{DB866D20-2C8E-4912-AE54-C0DE73A961D1}"/>
-    <hyperlink ref="F27" r:id="rId23" xr:uid="{E6BB6C09-7934-4350-BB7C-2F1AEEA03203}"/>
-    <hyperlink ref="F29" r:id="rId24" xr:uid="{DBB4A821-5C7C-42B3-B932-BE866252271E}"/>
-    <hyperlink ref="F28" r:id="rId25" xr:uid="{AB75C037-2E36-45AF-A0D6-5F0E44ED60B7}"/>
-    <hyperlink ref="F30" r:id="rId26" xr:uid="{6EB5851F-A799-4CAA-BF06-29C9C939DC49}"/>
-    <hyperlink ref="F31" r:id="rId27" xr:uid="{67A86030-580B-4839-9A7D-92E0AD0F6809}"/>
-    <hyperlink ref="F32" r:id="rId28" xr:uid="{23922AE4-F633-4A2F-BD2C-C8D90161DF16}"/>
-    <hyperlink ref="F33" r:id="rId29" xr:uid="{7F2317CC-0669-4473-A20D-F89D477FB146}"/>
-    <hyperlink ref="F34" r:id="rId30" xr:uid="{35473813-82B7-4BE4-8723-294547930526}"/>
-    <hyperlink ref="F35" r:id="rId31" xr:uid="{E837631F-D23E-4E81-A9BD-A5C5027968AC}"/>
-    <hyperlink ref="F36" r:id="rId32" xr:uid="{F5F9855D-7667-4092-8054-8787E6E8885C}"/>
-    <hyperlink ref="F37" r:id="rId33" xr:uid="{36E0E01F-166F-4EFF-9AF7-09B8F8475A02}"/>
-    <hyperlink ref="F39" r:id="rId34" xr:uid="{F9A1C182-1E7C-4BD4-96D5-04DE59F23C70}"/>
-    <hyperlink ref="F38" r:id="rId35" xr:uid="{0A42A0CD-2735-45A5-942D-90525AA1F2AD}"/>
-    <hyperlink ref="F40" r:id="rId36" xr:uid="{7100F2C7-7F95-49AE-8710-58734F4F3C32}"/>
-    <hyperlink ref="F42" r:id="rId37" xr:uid="{4794F883-D0CF-4EBF-9159-CA803800ED3F}"/>
-    <hyperlink ref="F41" r:id="rId38" xr:uid="{7473AD04-8192-4409-82E1-BBC5BF4849A1}"/>
-    <hyperlink ref="F43" r:id="rId39" xr:uid="{0B187283-6428-415D-8F47-537D14FC32A5}"/>
-    <hyperlink ref="F45" r:id="rId40" xr:uid="{26823081-21F9-43F3-BBE1-B4F0AF0C4E13}"/>
-    <hyperlink ref="F44" r:id="rId41" xr:uid="{7FB3CB1F-54FF-485E-AF21-372815835995}"/>
-    <hyperlink ref="F47" r:id="rId42" xr:uid="{E8030A24-33DB-434A-8744-0AC7A9EC4E74}"/>
-    <hyperlink ref="F46" r:id="rId43" xr:uid="{B6B2615C-E8EF-446A-82EF-80AF88FE9FFA}"/>
-    <hyperlink ref="F49" r:id="rId44" xr:uid="{2916DBE6-9929-4235-872D-7150CFE2A2D1}"/>
-    <hyperlink ref="F48" r:id="rId45" xr:uid="{72F45366-598E-4F39-AC3F-35F53F91739A}"/>
-    <hyperlink ref="F50" r:id="rId46" xr:uid="{6BF86666-31D7-40A2-B06C-122326A70B59}"/>
-    <hyperlink ref="F52" r:id="rId47" xr:uid="{16B85607-F5B2-493A-AF8F-14523DF78C5A}"/>
-    <hyperlink ref="F51" r:id="rId48" xr:uid="{7694C872-4185-4007-8C31-2899E3A39230}"/>
-    <hyperlink ref="F53" r:id="rId49" xr:uid="{6A0A716E-1109-42F8-BB98-A436A9B86004}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{90527381-36DF-4A90-999E-72A67B889E6C}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{1EF029AC-4F76-4CBB-8667-8BC81D53A3DF}"/>
+    <hyperlink ref="G26" r:id="rId21" xr:uid="{36D72442-02B1-43AE-9099-FA35E2EF38CE}"/>
+    <hyperlink ref="G25" r:id="rId22" xr:uid="{DB866D20-2C8E-4912-AE54-C0DE73A961D1}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{E6BB6C09-7934-4350-BB7C-2F1AEEA03203}"/>
+    <hyperlink ref="G29" r:id="rId24" xr:uid="{DBB4A821-5C7C-42B3-B932-BE866252271E}"/>
+    <hyperlink ref="G28" r:id="rId25" xr:uid="{AB75C037-2E36-45AF-A0D6-5F0E44ED60B7}"/>
+    <hyperlink ref="G30" r:id="rId26" xr:uid="{6EB5851F-A799-4CAA-BF06-29C9C939DC49}"/>
+    <hyperlink ref="G31" r:id="rId27" xr:uid="{67A86030-580B-4839-9A7D-92E0AD0F6809}"/>
+    <hyperlink ref="G32" r:id="rId28" xr:uid="{23922AE4-F633-4A2F-BD2C-C8D90161DF16}"/>
+    <hyperlink ref="G33" r:id="rId29" xr:uid="{7F2317CC-0669-4473-A20D-F89D477FB146}"/>
+    <hyperlink ref="G34" r:id="rId30" xr:uid="{35473813-82B7-4BE4-8723-294547930526}"/>
+    <hyperlink ref="G35" r:id="rId31" xr:uid="{E837631F-D23E-4E81-A9BD-A5C5027968AC}"/>
+    <hyperlink ref="G36" r:id="rId32" xr:uid="{F5F9855D-7667-4092-8054-8787E6E8885C}"/>
+    <hyperlink ref="G37" r:id="rId33" xr:uid="{36E0E01F-166F-4EFF-9AF7-09B8F8475A02}"/>
+    <hyperlink ref="G39" r:id="rId34" xr:uid="{F9A1C182-1E7C-4BD4-96D5-04DE59F23C70}"/>
+    <hyperlink ref="G38" r:id="rId35" xr:uid="{0A42A0CD-2735-45A5-942D-90525AA1F2AD}"/>
+    <hyperlink ref="G40" r:id="rId36" xr:uid="{7100F2C7-7F95-49AE-8710-58734F4F3C32}"/>
+    <hyperlink ref="G42" r:id="rId37" xr:uid="{4794F883-D0CF-4EBF-9159-CA803800ED3F}"/>
+    <hyperlink ref="G41" r:id="rId38" xr:uid="{7473AD04-8192-4409-82E1-BBC5BF4849A1}"/>
+    <hyperlink ref="G43" r:id="rId39" xr:uid="{0B187283-6428-415D-8F47-537D14FC32A5}"/>
+    <hyperlink ref="G45" r:id="rId40" xr:uid="{26823081-21F9-43F3-BBE1-B4F0AF0C4E13}"/>
+    <hyperlink ref="G44" r:id="rId41" xr:uid="{7FB3CB1F-54FF-485E-AF21-372815835995}"/>
+    <hyperlink ref="G47" r:id="rId42" xr:uid="{E8030A24-33DB-434A-8744-0AC7A9EC4E74}"/>
+    <hyperlink ref="G46" r:id="rId43" xr:uid="{B6B2615C-E8EF-446A-82EF-80AF88FE9FFA}"/>
+    <hyperlink ref="G49" r:id="rId44" xr:uid="{2916DBE6-9929-4235-872D-7150CFE2A2D1}"/>
+    <hyperlink ref="G48" r:id="rId45" xr:uid="{72F45366-598E-4F39-AC3F-35F53F91739A}"/>
+    <hyperlink ref="G50" r:id="rId46" xr:uid="{6BF86666-31D7-40A2-B06C-122326A70B59}"/>
+    <hyperlink ref="G52" r:id="rId47" xr:uid="{16B85607-F5B2-493A-AF8F-14523DF78C5A}"/>
+    <hyperlink ref="G51" r:id="rId48" xr:uid="{7694C872-4185-4007-8C31-2899E3A39230}"/>
+    <hyperlink ref="G53" r:id="rId49" xr:uid="{6A0A716E-1109-42F8-BB98-A436A9B86004}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 
@@ -2125,15 +2461,15 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2141,10 +2477,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2152,10 +2488,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2163,10 +2499,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2174,10 +2510,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -2185,10 +2521,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -2196,10 +2532,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -2207,10 +2543,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -2218,10 +2554,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -2229,10 +2565,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -2240,10 +2576,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -2251,10 +2587,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -2262,10 +2598,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -2273,10 +2609,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -2284,10 +2620,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -2295,10 +2631,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -2306,10 +2642,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -2317,10 +2653,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -2328,10 +2664,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -2339,10 +2675,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -2350,10 +2686,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -2361,10 +2697,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -2372,10 +2708,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -2383,10 +2719,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -2394,10 +2730,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -2405,10 +2741,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -2416,10 +2752,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -2427,10 +2763,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -2438,10 +2774,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -2449,10 +2785,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -2460,10 +2796,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <v>37</v>
@@ -2471,10 +2807,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33">
         <v>38</v>
@@ -2482,10 +2818,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34">
         <v>39</v>
@@ -2493,10 +2829,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2504,10 +2840,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2515,10 +2851,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -2526,10 +2862,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -2537,10 +2873,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -2548,10 +2884,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -2559,10 +2895,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41">
         <v>7</v>
@@ -2570,10 +2906,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42">
         <v>8</v>
@@ -2581,10 +2917,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43">
         <v>9</v>
@@ -2592,10 +2928,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44">
         <v>10</v>
@@ -2603,10 +2939,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45">
         <v>11</v>
@@ -2614,10 +2950,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46">
         <v>12</v>
@@ -2625,10 +2961,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>13</v>
@@ -2636,10 +2972,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>14</v>
@@ -2647,10 +2983,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49">
         <v>15</v>
@@ -2658,10 +2994,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C50">
         <v>16</v>
@@ -2669,10 +3005,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51">
         <v>17</v>
@@ -2680,10 +3016,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
         <v>58</v>
-      </c>
-      <c r="B52" t="s">
-        <v>59</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2691,10 +3027,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" t="s">
         <v>58</v>
-      </c>
-      <c r="B53" t="s">
-        <v>59</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -2702,10 +3038,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
         <v>58</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -2713,10 +3049,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
         <v>58</v>
-      </c>
-      <c r="B55" t="s">
-        <v>59</v>
       </c>
       <c r="C55">
         <v>4</v>
@@ -2724,10 +3060,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
         <v>58</v>
-      </c>
-      <c r="B56" t="s">
-        <v>59</v>
       </c>
       <c r="C56">
         <v>5</v>
@@ -2735,10 +3071,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
         <v>58</v>
-      </c>
-      <c r="B57" t="s">
-        <v>59</v>
       </c>
       <c r="C57">
         <v>6</v>
@@ -2746,10 +3082,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>58</v>
-      </c>
-      <c r="B58" t="s">
-        <v>59</v>
       </c>
       <c r="C58">
         <v>7</v>
@@ -2757,10 +3093,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
         <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>59</v>
       </c>
       <c r="C59">
         <v>8</v>
@@ -2768,10 +3104,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
         <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>59</v>
       </c>
       <c r="C60">
         <v>9</v>
@@ -2779,10 +3115,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" t="s">
         <v>58</v>
-      </c>
-      <c r="B61" t="s">
-        <v>59</v>
       </c>
       <c r="C61">
         <v>10</v>
@@ -2790,10 +3126,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" t="s">
         <v>58</v>
-      </c>
-      <c r="B62" t="s">
-        <v>59</v>
       </c>
       <c r="C62">
         <v>11</v>
@@ -2801,10 +3137,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" t="s">
         <v>58</v>
-      </c>
-      <c r="B63" t="s">
-        <v>59</v>
       </c>
       <c r="C63">
         <v>12</v>
@@ -2812,10 +3148,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64" t="s">
         <v>58</v>
-      </c>
-      <c r="B64" t="s">
-        <v>59</v>
       </c>
       <c r="C64">
         <v>13</v>
@@ -2823,10 +3159,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" t="s">
         <v>58</v>
-      </c>
-      <c r="B65" t="s">
-        <v>59</v>
       </c>
       <c r="C65">
         <v>14</v>
@@ -2834,10 +3170,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" t="s">
         <v>58</v>
-      </c>
-      <c r="B66" t="s">
-        <v>59</v>
       </c>
       <c r="C66">
         <v>15</v>
@@ -2845,10 +3181,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" t="s">
         <v>58</v>
-      </c>
-      <c r="B67" t="s">
-        <v>59</v>
       </c>
       <c r="C67">
         <v>16</v>
@@ -2856,10 +3192,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" t="s">
         <v>58</v>
-      </c>
-      <c r="B68" t="s">
-        <v>59</v>
       </c>
       <c r="C68">
         <v>17</v>
@@ -2867,10 +3203,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
         <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>69</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2878,10 +3214,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
         <v>68</v>
-      </c>
-      <c r="B70" t="s">
-        <v>69</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -2889,10 +3225,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" t="s">
         <v>68</v>
-      </c>
-      <c r="B71" t="s">
-        <v>69</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -2900,10 +3236,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" t="s">
         <v>68</v>
-      </c>
-      <c r="B72" t="s">
-        <v>69</v>
       </c>
       <c r="C72">
         <v>4</v>
@@ -2911,10 +3247,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" t="s">
         <v>68</v>
-      </c>
-      <c r="B73" t="s">
-        <v>69</v>
       </c>
       <c r="C73">
         <v>5</v>
@@ -2922,10 +3258,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" t="s">
         <v>68</v>
-      </c>
-      <c r="B74" t="s">
-        <v>69</v>
       </c>
       <c r="C74">
         <v>6</v>
@@ -2933,10 +3269,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" t="s">
         <v>68</v>
-      </c>
-      <c r="B75" t="s">
-        <v>69</v>
       </c>
       <c r="C75">
         <v>7</v>
@@ -2944,10 +3280,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" t="s">
         <v>68</v>
-      </c>
-      <c r="B76" t="s">
-        <v>69</v>
       </c>
       <c r="C76">
         <v>8</v>
@@ -2955,10 +3291,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
         <v>68</v>
-      </c>
-      <c r="B77" t="s">
-        <v>69</v>
       </c>
       <c r="C77">
         <v>9</v>
@@ -2966,10 +3302,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="s">
         <v>68</v>
-      </c>
-      <c r="B78" t="s">
-        <v>69</v>
       </c>
       <c r="C78">
         <v>10</v>
@@ -2977,10 +3313,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
         <v>68</v>
-      </c>
-      <c r="B79" t="s">
-        <v>69</v>
       </c>
       <c r="C79">
         <v>11</v>
@@ -2988,10 +3324,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80" t="s">
         <v>68</v>
-      </c>
-      <c r="B80" t="s">
-        <v>69</v>
       </c>
       <c r="C80">
         <v>12</v>
@@ -2999,10 +3335,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" t="s">
         <v>68</v>
-      </c>
-      <c r="B81" t="s">
-        <v>69</v>
       </c>
       <c r="C81">
         <v>13</v>
@@ -3010,10 +3346,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82" t="s">
         <v>68</v>
-      </c>
-      <c r="B82" t="s">
-        <v>69</v>
       </c>
       <c r="C82">
         <v>14</v>
@@ -3021,10 +3357,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" t="s">
         <v>68</v>
-      </c>
-      <c r="B83" t="s">
-        <v>69</v>
       </c>
       <c r="C83">
         <v>15</v>
@@ -3032,10 +3368,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" t="s">
         <v>68</v>
-      </c>
-      <c r="B84" t="s">
-        <v>69</v>
       </c>
       <c r="C84">
         <v>16</v>
@@ -3043,10 +3379,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" t="s">
         <v>68</v>
-      </c>
-      <c r="B85" t="s">
-        <v>69</v>
       </c>
       <c r="C85">
         <v>17</v>
@@ -3054,10 +3390,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" t="s">
         <v>68</v>
-      </c>
-      <c r="B86" t="s">
-        <v>69</v>
       </c>
       <c r="C86">
         <v>18</v>
@@ -3065,10 +3401,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" t="s">
         <v>68</v>
-      </c>
-      <c r="B87" t="s">
-        <v>69</v>
       </c>
       <c r="C87">
         <v>19</v>
@@ -3076,10 +3412,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88" t="s">
         <v>196</v>
-      </c>
-      <c r="B88" t="s">
-        <v>197</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -3087,10 +3423,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>195</v>
+      </c>
+      <c r="B89" t="s">
         <v>196</v>
-      </c>
-      <c r="B89" t="s">
-        <v>197</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -3098,10 +3434,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -3109,10 +3445,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -3120,10 +3456,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C92">
         <v>3</v>
@@ -3131,10 +3467,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C93">
         <v>4</v>
@@ -3142,10 +3478,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C94">
         <v>5</v>
@@ -3153,10 +3489,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C95">
         <v>6</v>
@@ -3164,10 +3500,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C96">
         <v>7</v>
@@ -3175,10 +3511,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C97">
         <v>8</v>
@@ -3186,10 +3522,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C98">
         <v>9</v>
@@ -3197,10 +3533,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C99">
         <v>10</v>
@@ -3208,10 +3544,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C100">
         <v>11</v>
@@ -3219,10 +3555,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C101">
         <v>12</v>
@@ -3230,10 +3566,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C102">
         <v>13</v>
@@ -3241,10 +3577,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C103">
         <v>14</v>
@@ -3252,10 +3588,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C104">
         <v>15</v>
@@ -3263,10 +3599,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C105">
         <v>16</v>
@@ -3274,10 +3610,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B106" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C106">
         <v>17</v>
@@ -3285,10 +3621,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C107">
         <v>18</v>
@@ -3296,10 +3632,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B108" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C108">
         <v>19</v>
@@ -3307,10 +3643,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C109">
         <v>20</v>
@@ -3318,10 +3654,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B110" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C110">
         <v>21</v>
@@ -3329,10 +3665,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B111" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C111">
         <v>22</v>
@@ -3340,10 +3676,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B112" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C112">
         <v>23</v>
@@ -3351,10 +3687,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C113">
         <v>24</v>
@@ -3362,10 +3698,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B114" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C114">
         <v>25</v>
@@ -3373,10 +3709,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B115" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C115">
         <v>26</v>
@@ -3384,10 +3720,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B116" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C116">
         <v>27</v>
@@ -3395,10 +3731,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C117">
         <v>28</v>
@@ -3406,10 +3742,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B118" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C118">
         <v>29</v>
@@ -3417,10 +3753,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B119" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -3428,10 +3764,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B120" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C120">
         <v>2</v>
@@ -3439,10 +3775,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B121" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C121">
         <v>3</v>
@@ -3450,10 +3786,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B122" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C122">
         <v>4</v>
@@ -3461,10 +3797,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B123" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C123">
         <v>5</v>
@@ -3472,10 +3808,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C124">
         <v>6</v>
@@ -3483,10 +3819,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C125">
         <v>7</v>
@@ -3494,10 +3830,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C126">
         <v>8</v>
@@ -3505,10 +3841,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B127" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C127">
         <v>9</v>
@@ -3516,10 +3852,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B128" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C128">
         <v>10</v>
@@ -3527,10 +3863,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B129" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C129">
         <v>11</v>
@@ -3538,10 +3874,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B130" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C130">
         <v>12</v>
@@ -3549,10 +3885,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B131" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C131">
         <v>13</v>
@@ -3560,10 +3896,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B132" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C132">
         <v>14</v>
@@ -3571,10 +3907,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B133" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C133">
         <v>15</v>
@@ -3582,10 +3918,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B134" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C134">
         <v>16</v>
@@ -3593,10 +3929,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B135" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C135">
         <v>17</v>
@@ -3604,10 +3940,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B136" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C136">
         <v>18</v>
@@ -3615,10 +3951,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B137" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C137">
         <v>19</v>
@@ -3626,10 +3962,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B138" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C138">
         <v>20</v>
@@ -3637,10 +3973,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B139" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C139">
         <v>21</v>
@@ -3648,10 +3984,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B140" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C140">
         <v>22</v>
@@ -3659,10 +3995,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B141" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C141">
         <v>23</v>
@@ -3670,10 +4006,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B142" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C142">
         <v>24</v>
@@ -3681,10 +4017,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B143" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C143">
         <v>25</v>
@@ -3692,10 +4028,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B144" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C144">
         <v>26</v>
@@ -3703,10 +4039,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B145" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C145">
         <v>27</v>
@@ -3714,10 +4050,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C146">
         <v>28</v>
@@ -3725,10 +4061,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B147" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C147">
         <v>29</v>
@@ -3736,10 +4072,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B148" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C148">
         <v>30</v>
@@ -3747,10 +4083,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B149" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C149">
         <v>31</v>
@@ -3758,10 +4094,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B150" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C150">
         <v>32</v>
@@ -3769,10 +4105,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B151" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C151">
         <v>33</v>
@@ -3780,10 +4116,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B152" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C152">
         <v>34</v>
@@ -3791,10 +4127,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B153" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C153">
         <v>35</v>
@@ -3802,10 +4138,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B154" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C154">
         <v>36</v>
@@ -3813,10 +4149,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B155" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C155">
         <v>37</v>
@@ -3824,10 +4160,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B156" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C156">
         <v>38</v>
@@ -3835,10 +4171,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B157" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C157">
         <v>39</v>
@@ -3846,10 +4182,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B158" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C158">
         <v>40</v>
@@ -3857,10 +4193,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B159" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C159">
         <v>41</v>
@@ -3868,10 +4204,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B160" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C160">
         <v>42</v>
@@ -3879,10 +4215,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B161" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C161">
         <v>43</v>
@@ -3890,10 +4226,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B162" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C162">
         <v>44</v>
@@ -3901,10 +4237,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B163" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C163">
         <v>45</v>
@@ -3912,10 +4248,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B164" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C164">
         <v>46</v>
@@ -3923,10 +4259,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B165" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C165">
         <v>47</v>
@@ -3934,10 +4270,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B166" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C166">
         <v>48</v>
@@ -3945,10 +4281,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B167" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C167">
         <v>49</v>
@@ -3956,10 +4292,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B168" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C168">
         <v>50</v>
@@ -3967,10 +4303,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B169" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C169">
         <v>51</v>
@@ -3978,10 +4314,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B170" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C170">
         <v>52</v>
@@ -3989,10 +4325,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B171" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C171">
         <v>53</v>
@@ -4000,10 +4336,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B172" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C172">
         <v>54</v>
@@ -4011,10 +4347,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B173" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C173">
         <v>55</v>
@@ -4022,10 +4358,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B174" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C174">
         <v>56</v>

</xml_diff>